<commit_message>
Mostly finished intro. Working on plots
</commit_message>
<xml_diff>
--- a/plots/matrix.xlsx
+++ b/plots/matrix.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmccombs/projects/phi_benchmarking/R_benchmarking/WhitePaper/PEARC17/plots/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scamicha/ResearchGit/PaperWriting/PEARC17/plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-30100" yWindow="1440" windowWidth="28160" windowHeight="16880" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1440" windowWidth="28160" windowHeight="16880" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="cross(20000)" sheetId="1" r:id="rId1"/>
     <sheet name="matmat(20000)" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="14">
   <si>
     <t>Num Threads</t>
   </si>
@@ -44,6 +45,33 @@
   <si>
     <t>SNB Scaling</t>
   </si>
+  <si>
+    <t>KNL</t>
+  </si>
+  <si>
+    <t>SNB</t>
+  </si>
+  <si>
+    <t>cross</t>
+  </si>
+  <si>
+    <t>matmat</t>
+  </si>
+  <si>
+    <t>threads</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>processor</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>scaling</t>
+  </si>
 </sst>
 </file>
 
@@ -52,7 +80,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -83,6 +111,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -101,12 +136,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -120,10 +159,20 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -401,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -633,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -857,4 +906,614 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <v>217.5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>113.1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.9227695569037808</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6">
+        <v>62.16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3.4990769824767436</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6">
+        <v>33.270000000000003</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2">
+        <v>6.5374535960976692</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>16</v>
+      </c>
+      <c r="B6" s="6">
+        <v>18.59</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2">
+        <v>11.702941614829298</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>34</v>
+      </c>
+      <c r="B7" s="6">
+        <v>10.85</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2">
+        <v>20.054723157069752</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>66</v>
+      </c>
+      <c r="B8" s="6">
+        <v>8.0389999999999997</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2">
+        <v>27.057301466357742</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>68</v>
+      </c>
+      <c r="B9" s="6">
+        <v>8.1790000000000003</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="2">
+        <v>26.592920894974934</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>136</v>
+      </c>
+      <c r="B10" s="6">
+        <v>15.2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2">
+        <v>14.308970099667775</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>204</v>
+      </c>
+      <c r="B11" s="6">
+        <v>16.45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="2">
+        <v>13.223600494402708</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>272</v>
+      </c>
+      <c r="B12" s="6">
+        <v>18.04</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="2">
+        <v>12.057570507934308</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2">
+        <v>358.91800000000001</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2">
+        <v>180.8015</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1.9851494594901038</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>4</v>
+      </c>
+      <c r="B15" s="2">
+        <v>93.045119999999997</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="2">
+        <v>3.8574618421686169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2">
+        <v>49.255870000000002</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="2">
+        <v>7.286806628326735</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2">
+        <v>34.684620000000002</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="2">
+        <v>10.348044752976968</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2">
+        <v>27.503250000000001</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="2">
+        <v>13.050021361111869</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19" s="4">
+        <v>155.02000000000001</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>2</v>
+      </c>
+      <c r="B20" s="4">
+        <v>92.993750000000006</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1.666993749579945</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>4</v>
+      </c>
+      <c r="B21" s="4">
+        <v>49.512500000000003</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="4">
+        <v>3.1309265337036103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>8</v>
+      </c>
+      <c r="B22" s="4">
+        <v>25.573619999999998</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="4">
+        <v>6.0617151580417641</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>16</v>
+      </c>
+      <c r="B23" s="4">
+        <v>13.5215</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="4">
+        <v>11.464704359723404</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>34</v>
+      </c>
+      <c r="B24" s="4">
+        <v>6.2942499999999999</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="4">
+        <v>24.628827898478772</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>66</v>
+      </c>
+      <c r="B25" s="4">
+        <v>4.1136249999999999</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="4">
+        <v>37.684523990397764</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>68</v>
+      </c>
+      <c r="B26" s="4">
+        <v>3.9235000000000002</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="4">
+        <v>39.510641009302915</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>136</v>
+      </c>
+      <c r="B27" s="4">
+        <v>4.7522500000000001</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="4">
+        <v>32.620337734757221</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>204</v>
+      </c>
+      <c r="B28" s="4">
+        <v>8.4239999999999995</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="4">
+        <v>18.40218423551757</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>272</v>
+      </c>
+      <c r="B29" s="4">
+        <v>10.69112</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="4">
+        <v>14.499884015893565</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>1</v>
+      </c>
+      <c r="B30" s="4">
+        <v>244.22049999999999</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>2</v>
+      </c>
+      <c r="B31" s="4">
+        <v>125.413</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="4">
+        <v>1.9473300216086051</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>4</v>
+      </c>
+      <c r="B32" s="4">
+        <v>64.391249999999999</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="4">
+        <v>3.7927591093510373</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>8</v>
+      </c>
+      <c r="B33" s="4">
+        <v>34.510750000000002</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="4">
+        <v>7.0766500293386834</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>12</v>
+      </c>
+      <c r="B34" s="4">
+        <v>24.028500000000001</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="4">
+        <v>10.163784672368228</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>16</v>
+      </c>
+      <c r="B35" s="4">
+        <v>19.791630000000001</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="4">
+        <v>12.339584965967935</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>